<commit_message>
Added missing THT components
</commit_message>
<xml_diff>
--- a/cam/RP2040-Eins-20231007-JLCPCB-CPL.xlsx
+++ b/cam/RP2040-Eins-20231007-JLCPCB-CPL.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\KiCad\7.0\projects\RP2040-Eins\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B102122B-8E83-4D40-AEC2-2EFC8EF59332}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{39140691-194C-4441-B0F1-CEE910D2A92D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="8904" windowWidth="14040" windowHeight="14292" xr2:uid="{AB60BF64-F087-4623-A932-7FC873342513}"/>
+    <workbookView xWindow="13992" yWindow="2556" windowWidth="14040" windowHeight="14292" xr2:uid="{D2A07367-EB26-4D3C-95B3-13C76D9B899A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="RP2040_Eins_top_pos" localSheetId="0">Sheet1!$A$1:$E$52</definedName>
+    <definedName name="RP2040_Eins_top_pos" localSheetId="0">Sheet1!$A$1:$E$62</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{AA479360-FE20-419A-8E5C-151FA1D30827}" name="RP2040-Eins-top-pos" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="1" xr16:uid="{BA9BFB1F-A681-4651-AD66-8BEFF8531739}" name="RP2040-Eins-top-pos" type="6" refreshedVersion="8" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\AG\Documents\KiCad\7.0\projects\RP2040-Eins\cam\RP2040-Eins-top-pos.csv" tab="0" comma="1">
       <textFields count="7">
         <textField/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="67">
   <si>
     <t>C1</t>
   </si>
@@ -132,6 +132,30 @@
     <t>FB2</t>
   </si>
   <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>J8</t>
+  </si>
+  <si>
+    <t>J9</t>
+  </si>
+  <si>
     <t>J10</t>
   </si>
   <si>
@@ -184,6 +208,12 @@
   </si>
   <si>
     <t>R15</t>
+  </si>
+  <si>
+    <t>SW1</t>
+  </si>
+  <si>
+    <t>SW2</t>
   </si>
   <si>
     <t>U1</t>
@@ -279,7 +309,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="RP2040-Eins-top-pos" connectionId="1" xr16:uid="{08180941-1627-4116-BC7B-B2F5E0FE501C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="RP2040-Eins-top-pos" connectionId="1" xr16:uid="{0A901281-81A5-40EA-9926-E9F1ADE38999}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -578,37 +608,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA10E596-FBF1-47B0-A499-A6942A729FD6}">
-  <dimension ref="A1:E52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C0E679-E78B-48F3-874D-D3B284C2D2EB}">
+  <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.77734375" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="6.44140625" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1075,16 +1105,16 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>129.54</v>
+        <v>137.572</v>
       </c>
       <c r="C29">
-        <v>-88.9</v>
+        <v>-119.38</v>
       </c>
       <c r="D29" t="s">
         <v>1</v>
       </c>
       <c r="E29">
-        <v>-90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1092,16 +1122,16 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>146.05000000000001</v>
+        <v>190.495</v>
       </c>
       <c r="C30">
-        <v>-106.172</v>
+        <v>-96.52</v>
       </c>
       <c r="D30" t="s">
         <v>1</v>
       </c>
       <c r="E30">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1109,10 +1139,10 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>139.512</v>
+        <v>177.8</v>
       </c>
       <c r="C31">
-        <v>-105.9965</v>
+        <v>-124.46</v>
       </c>
       <c r="D31" t="s">
         <v>1</v>
@@ -1126,16 +1156,16 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>133.35</v>
+        <v>154.95500000000001</v>
       </c>
       <c r="C32">
-        <v>-102.87</v>
+        <v>-124.435</v>
       </c>
       <c r="D32" t="s">
         <v>1</v>
       </c>
       <c r="E32">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1143,16 +1173,16 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>181.61</v>
+        <v>190.5</v>
       </c>
       <c r="C33">
-        <v>-102.108</v>
+        <v>-85.07</v>
       </c>
       <c r="D33" t="s">
         <v>1</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1160,10 +1190,10 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>181.61</v>
+        <v>191.14500000000001</v>
       </c>
       <c r="C34">
-        <v>-103.378</v>
+        <v>-106.67</v>
       </c>
       <c r="D34" t="s">
         <v>1</v>
@@ -1177,16 +1207,16 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>181.61</v>
+        <v>190.5</v>
       </c>
       <c r="C35">
-        <v>-104.648</v>
+        <v>-76.2</v>
       </c>
       <c r="D35" t="s">
         <v>1</v>
       </c>
       <c r="E35">
-        <v>0</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1194,16 +1224,16 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>181.61</v>
+        <v>168.626</v>
       </c>
       <c r="C36">
-        <v>-89.915999999999997</v>
+        <v>-76.224999999999994</v>
       </c>
       <c r="D36" t="s">
         <v>1</v>
       </c>
       <c r="E36">
-        <v>180</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1211,16 +1241,16 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>133.35</v>
+        <v>129.54</v>
       </c>
       <c r="C37">
-        <v>-107.95</v>
+        <v>-88.9</v>
       </c>
       <c r="D37" t="s">
         <v>1</v>
       </c>
       <c r="E37">
-        <v>180</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1228,10 +1258,10 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>173.99</v>
+        <v>146.05000000000001</v>
       </c>
       <c r="C38">
-        <v>-107.95</v>
+        <v>-106.172</v>
       </c>
       <c r="D38" t="s">
         <v>1</v>
@@ -1245,10 +1275,10 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>142.74799999999999</v>
+        <v>139.512</v>
       </c>
       <c r="C39">
-        <v>-106.934</v>
+        <v>-105.9965</v>
       </c>
       <c r="D39" t="s">
         <v>1</v>
@@ -1262,16 +1292,16 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>142.74799999999999</v>
+        <v>133.35</v>
       </c>
       <c r="C40">
-        <v>-104.902</v>
+        <v>-102.87</v>
       </c>
       <c r="D40" t="s">
         <v>1</v>
       </c>
       <c r="E40">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1279,16 +1309,16 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>136.90600000000001</v>
+        <v>181.61</v>
       </c>
       <c r="C41">
-        <v>-85.597999999999999</v>
+        <v>-102.108</v>
       </c>
       <c r="D41" t="s">
         <v>1</v>
       </c>
       <c r="E41">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1296,16 +1326,16 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>136.90600000000001</v>
+        <v>181.61</v>
       </c>
       <c r="C42">
-        <v>-92.2</v>
+        <v>-103.378</v>
       </c>
       <c r="D42" t="s">
         <v>1</v>
       </c>
       <c r="E42">
-        <v>-90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1313,10 +1343,10 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>130.30199999999999</v>
+        <v>181.61</v>
       </c>
       <c r="C43">
-        <v>-82.55</v>
+        <v>-104.648</v>
       </c>
       <c r="D43" t="s">
         <v>1</v>
@@ -1330,16 +1360,16 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>175.26</v>
+        <v>181.61</v>
       </c>
       <c r="C44">
-        <v>-107.95</v>
+        <v>-89.915999999999997</v>
       </c>
       <c r="D44" t="s">
         <v>1</v>
       </c>
       <c r="E44">
-        <v>-90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1347,7 +1377,7 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>176.53</v>
+        <v>133.35</v>
       </c>
       <c r="C45">
         <v>-107.95</v>
@@ -1356,7 +1386,7 @@
         <v>1</v>
       </c>
       <c r="E45">
-        <v>-90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1364,7 +1394,7 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>177.8</v>
+        <v>173.99</v>
       </c>
       <c r="C46">
         <v>-107.95</v>
@@ -1373,7 +1403,7 @@
         <v>1</v>
       </c>
       <c r="E46">
-        <v>-90</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1381,16 +1411,16 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>153.66999999999999</v>
+        <v>142.74799999999999</v>
       </c>
       <c r="C47">
-        <v>-100.33</v>
+        <v>-106.934</v>
       </c>
       <c r="D47" t="s">
         <v>1</v>
       </c>
       <c r="E47">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1398,10 +1428,10 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>168.91</v>
+        <v>142.74799999999999</v>
       </c>
       <c r="C48">
-        <v>-95.25</v>
+        <v>-104.902</v>
       </c>
       <c r="D48" t="s">
         <v>1</v>
@@ -1415,16 +1445,16 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>146.489</v>
+        <v>136.90600000000001</v>
       </c>
       <c r="C49">
-        <v>-112.047</v>
+        <v>-85.597999999999999</v>
       </c>
       <c r="D49" t="s">
         <v>1</v>
       </c>
       <c r="E49">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1432,16 +1462,16 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>153.66999999999999</v>
+        <v>136.90600000000001</v>
       </c>
       <c r="C50">
-        <v>-100.33</v>
+        <v>-92.2</v>
       </c>
       <c r="D50" t="s">
         <v>1</v>
       </c>
       <c r="E50">
-        <v>180</v>
+        <v>-90</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1449,10 +1479,10 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>157.66499999999999</v>
+        <v>130.30199999999999</v>
       </c>
       <c r="C51">
-        <v>-112.047</v>
+        <v>-82.55</v>
       </c>
       <c r="D51" t="s">
         <v>1</v>
@@ -1466,15 +1496,185 @@
         <v>51</v>
       </c>
       <c r="B52">
+        <v>175.26</v>
+      </c>
+      <c r="C52">
+        <v>-107.95</v>
+      </c>
+      <c r="D52" t="s">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+      <c r="B53">
+        <v>176.53</v>
+      </c>
+      <c r="C53">
+        <v>-107.95</v>
+      </c>
+      <c r="D53" t="s">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>177.8</v>
+      </c>
+      <c r="C54">
+        <v>-107.95</v>
+      </c>
+      <c r="D54" t="s">
+        <v>1</v>
+      </c>
+      <c r="E54">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+      <c r="B55">
+        <v>168.91</v>
+      </c>
+      <c r="C55">
+        <v>-107.95</v>
+      </c>
+      <c r="D55" t="s">
+        <v>1</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+      <c r="B56">
+        <v>133.35</v>
+      </c>
+      <c r="C56">
+        <v>-77.47</v>
+      </c>
+      <c r="D56" t="s">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+      <c r="B57">
+        <v>153.66999999999999</v>
+      </c>
+      <c r="C57">
+        <v>-100.33</v>
+      </c>
+      <c r="D57" t="s">
+        <v>1</v>
+      </c>
+      <c r="E57">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+      <c r="B58">
+        <v>168.91</v>
+      </c>
+      <c r="C58">
+        <v>-95.25</v>
+      </c>
+      <c r="D58" t="s">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>146.489</v>
+      </c>
+      <c r="C59">
+        <v>-112.047</v>
+      </c>
+      <c r="D59" t="s">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+      <c r="B60">
+        <v>153.66999999999999</v>
+      </c>
+      <c r="C60">
+        <v>-100.33</v>
+      </c>
+      <c r="D60" t="s">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+      <c r="B61">
+        <v>157.66499999999999</v>
+      </c>
+      <c r="C61">
+        <v>-112.047</v>
+      </c>
+      <c r="D61" t="s">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62">
         <v>181.61</v>
       </c>
-      <c r="C52">
+      <c r="C62">
         <v>-96.52</v>
       </c>
-      <c r="D52" t="s">
-        <v>1</v>
-      </c>
-      <c r="E52">
+      <c r="D62" t="s">
+        <v>1</v>
+      </c>
+      <c r="E62">
         <v>-90</v>
       </c>
     </row>

</xml_diff>